<commit_message>
Changes for OM and PM - IGD targets weren't being met
This commit does two main things:
- recommits the changes I made yesterday at 10:36 am as these were lost:
"New input DMIs for Ops mode and MRM demo. For the ops mode demo, we need to input a bunch of values for both MRM and single mode.
Instead of taking the time to do that, I set up a DMI that brings in the appropriate data.
The source is an excel sheet KPOM_OM_InputsForTesting.xlsx in the Database folder.

- Reorders Rule 2 to become rule 4 and edits to correctly account for the lag.
It assumed a three day lag but we removed the physical lag.  Now we use the physical lag value.
</commit_message>
<xml_diff>
--- a/Database/KPOM_OM_InputsForTesting.xlsx
+++ b/Database/KPOM_OM_InputsForTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\riverware\staff\neumannd\KROM\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151EE1B6-7E33-46E7-88DA-E12D5D785E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1356399-75F2-4DAC-869D-67BDA4B0C74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="2790" windowWidth="70215" windowHeight="16125" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="1860" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>David Neumann:</t>
         </r>
@@ -56,7 +56,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Run 1</t>
@@ -71,7 +71,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>David Neumann:</t>
         </r>
@@ -80,7 +80,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Run 5</t>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="134">
   <si>
     <t>EWA.EWA May June Augment Release</t>
   </si>
@@ -476,6 +476,24 @@
   </si>
   <si>
     <t>MRM Dashboard.Agricultural Date Settings.Short</t>
+  </si>
+  <si>
+    <t>We should replace "Percentile" to "POE", "EP", or something that indicates exceedance instead of percentile</t>
+  </si>
+  <si>
+    <t>! median accretion</t>
+  </si>
+  <si>
+    <t>! 50% exceedance scenario</t>
+  </si>
+  <si>
+    <t>! 75% exceedance scenario</t>
+  </si>
+  <si>
+    <t>! 25% exceedance scenario</t>
+  </si>
+  <si>
+    <t>Nan</t>
   </si>
 </sst>
 </file>
@@ -486,7 +504,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -500,17 +518,23 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,6 +550,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -745,6 +775,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -754,20 +809,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,6 +830,255 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C8A6BB6-7C7C-44E9-AA3B-E4A2F3E3968E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8982075" y="171450"/>
+          <a:ext cx="247650" cy="2628900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E691EA-8BD0-4B6C-A2A8-7284122758D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9324975" y="180975"/>
+          <a:ext cx="2457450" cy="2600325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79EB9EF1-310B-44DF-A2BD-4D4DF8232C12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8543925" y="9525"/>
+          <a:ext cx="676275" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27117716-AE17-4C08-8405-FDA568F4AA5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11458575" y="9525"/>
+          <a:ext cx="676275" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1086,7 +1381,7 @@
   <dimension ref="A1:AO35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1100,12 +1395,10 @@
     <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -1134,68 +1427,68 @@
   <sheetData>
     <row r="1" spans="1:41">
       <c r="A1" s="8"/>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="48" t="s">
         <v>41</v>
       </c>
       <c r="C1" s="8"/>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="47"/>
       <c r="M1" s="8"/>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="38"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="20" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="8"/>
-      <c r="T1" s="37" t="s">
+      <c r="T1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="37"/>
+      <c r="U1" s="46"/>
       <c r="V1" s="8"/>
-      <c r="W1" s="37" t="s">
+      <c r="W1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="38"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="47"/>
       <c r="Z1" s="8"/>
-      <c r="AA1" s="37" t="s">
+      <c r="AA1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="38"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="47"/>
       <c r="AD1" s="8"/>
-      <c r="AE1" s="37" t="s">
+      <c r="AE1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="38"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="47"/>
       <c r="AH1" s="8"/>
-      <c r="AI1" s="37" t="s">
+      <c r="AI1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="38"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="47"/>
       <c r="AL1" s="8"/>
-      <c r="AM1" s="37" t="s">
+      <c r="AM1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="38"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="47"/>
     </row>
     <row r="2" spans="1:41">
       <c r="A2" s="9"/>
@@ -1331,13 +1624,13 @@
         <v>44257</v>
       </c>
       <c r="J3" s="30">
-        <v>102000</v>
+        <v>500000</v>
       </c>
       <c r="K3" s="30">
-        <v>81000</v>
+        <v>430000</v>
       </c>
       <c r="L3" s="31">
-        <v>61000</v>
+        <v>355000</v>
       </c>
       <c r="M3" s="17" t="s">
         <v>23</v>
@@ -1346,13 +1639,13 @@
         <v>44257</v>
       </c>
       <c r="O3" s="30">
-        <v>110614</v>
+        <v>500302</v>
       </c>
       <c r="P3" s="30">
-        <v>94469</v>
+        <v>421760</v>
       </c>
       <c r="Q3" s="31">
-        <v>85043</v>
+        <v>392986</v>
       </c>
       <c r="R3" s="16"/>
       <c r="S3" s="14" t="s">
@@ -1773,6 +2066,9 @@
       </c>
       <c r="C16" s="5"/>
       <c r="E16" s="7"/>
+      <c r="J16" s="42" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="12" t="s">
@@ -1935,6 +2231,7 @@
     <mergeCell ref="AA1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1942,11 +2239,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C520"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B236" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B194" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F241" sqref="F241"/>
+      <selection pane="bottomRight" activeCell="H196" sqref="H196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4173,8 +4470,8 @@
       <c r="B198" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C198" s="40">
-        <v>0</v>
+      <c r="C198" s="49" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -4185,7 +4482,7 @@
       <c r="B199" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C199" s="41">
+      <c r="C199" s="38">
         <v>5700</v>
       </c>
     </row>
@@ -4197,7 +4494,7 @@
       <c r="B200" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C200" s="40">
+      <c r="C200" s="37">
         <v>5600</v>
       </c>
     </row>
@@ -4209,7 +4506,7 @@
       <c r="B201" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C201" s="40">
+      <c r="C201" s="37">
         <v>5500</v>
       </c>
     </row>
@@ -4221,8 +4518,8 @@
       <c r="B202" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C202" s="42">
-        <v>0</v>
+      <c r="C202" s="50" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -4266,7 +4563,7 @@
         <f t="shared" si="0"/>
         <v>44308.999305555553</v>
       </c>
-      <c r="B206" s="43">
+      <c r="B206" s="39">
         <v>0</v>
       </c>
       <c r="C206" s="1" t="s">
@@ -4278,7 +4575,7 @@
         <f t="shared" si="0"/>
         <v>44309.999305555553</v>
       </c>
-      <c r="B207" s="44">
+      <c r="B207" s="40">
         <v>480</v>
       </c>
       <c r="C207" s="1" t="s">
@@ -4290,7 +4587,7 @@
         <f t="shared" si="0"/>
         <v>44310.999305555553</v>
       </c>
-      <c r="B208" s="44">
+      <c r="B208" s="40">
         <v>480</v>
       </c>
       <c r="C208" s="1" t="s">
@@ -4302,7 +4599,7 @@
         <f t="shared" si="0"/>
         <v>44311.999305555553</v>
       </c>
-      <c r="B209" s="44">
+      <c r="B209" s="40">
         <v>480</v>
       </c>
       <c r="C209" s="1" t="s">
@@ -4314,7 +4611,7 @@
         <f t="shared" si="0"/>
         <v>44312.999305555553</v>
       </c>
-      <c r="B210" s="44">
+      <c r="B210" s="40">
         <v>480</v>
       </c>
       <c r="C210" s="1" t="s">
@@ -4326,7 +4623,7 @@
         <f t="shared" si="0"/>
         <v>44313.999305555553</v>
       </c>
-      <c r="B211" s="44">
+      <c r="B211" s="40">
         <v>480</v>
       </c>
       <c r="C211" s="1" t="s">
@@ -4338,7 +4635,7 @@
         <f t="shared" si="0"/>
         <v>44314.999305555553</v>
       </c>
-      <c r="B212" s="44">
+      <c r="B212" s="40">
         <v>480</v>
       </c>
       <c r="C212" s="1" t="s">
@@ -4350,7 +4647,7 @@
         <f t="shared" si="0"/>
         <v>44315.999305555553</v>
       </c>
-      <c r="B213" s="44">
+      <c r="B213" s="40">
         <v>480</v>
       </c>
       <c r="C213" s="1" t="s">
@@ -4362,7 +4659,7 @@
         <f t="shared" si="0"/>
         <v>44316.999305555553</v>
       </c>
-      <c r="B214" s="44">
+      <c r="B214" s="40">
         <v>480</v>
       </c>
       <c r="C214" s="1" t="s">
@@ -4374,7 +4671,7 @@
         <f t="shared" si="0"/>
         <v>44317.999305555553</v>
       </c>
-      <c r="B215" s="44">
+      <c r="B215" s="40">
         <v>480</v>
       </c>
       <c r="C215" s="1" t="s">
@@ -4386,7 +4683,7 @@
         <f t="shared" si="0"/>
         <v>44318.999305555553</v>
       </c>
-      <c r="B216" s="44">
+      <c r="B216" s="40">
         <v>480</v>
       </c>
       <c r="C216" s="1" t="s">
@@ -4398,7 +4695,7 @@
         <f t="shared" si="0"/>
         <v>44319.999305555553</v>
       </c>
-      <c r="B217" s="44">
+      <c r="B217" s="40">
         <v>480</v>
       </c>
       <c r="C217" s="1" t="s">
@@ -4410,7 +4707,7 @@
         <f t="shared" si="0"/>
         <v>44320.999305555553</v>
       </c>
-      <c r="B218" s="44">
+      <c r="B218" s="40">
         <v>480</v>
       </c>
       <c r="C218" s="1" t="s">
@@ -4422,7 +4719,7 @@
         <f t="shared" ref="A219:A282" si="1">A218+1</f>
         <v>44321.999305555553</v>
       </c>
-      <c r="B219" s="44">
+      <c r="B219" s="40">
         <v>480</v>
       </c>
       <c r="C219" s="1" t="s">
@@ -4434,7 +4731,7 @@
         <f t="shared" si="1"/>
         <v>44322.999305555553</v>
       </c>
-      <c r="B220" s="44">
+      <c r="B220" s="40">
         <v>480</v>
       </c>
       <c r="C220" s="1" t="s">
@@ -4446,7 +4743,7 @@
         <f t="shared" si="1"/>
         <v>44323.999305555553</v>
       </c>
-      <c r="B221" s="44">
+      <c r="B221" s="40">
         <v>480</v>
       </c>
       <c r="C221" s="1" t="s">
@@ -4458,7 +4755,7 @@
         <f t="shared" si="1"/>
         <v>44324.999305555553</v>
       </c>
-      <c r="B222" s="44">
+      <c r="B222" s="40">
         <v>480</v>
       </c>
       <c r="C222" s="1" t="s">
@@ -4470,7 +4767,7 @@
         <f t="shared" si="1"/>
         <v>44325.999305555553</v>
       </c>
-      <c r="B223" s="44">
+      <c r="B223" s="40">
         <v>480</v>
       </c>
       <c r="C223" s="1" t="s">
@@ -4482,7 +4779,7 @@
         <f t="shared" si="1"/>
         <v>44326.999305555553</v>
       </c>
-      <c r="B224" s="44">
+      <c r="B224" s="40">
         <v>480</v>
       </c>
       <c r="C224" s="1" t="s">
@@ -4494,7 +4791,7 @@
         <f t="shared" si="1"/>
         <v>44327.999305555553</v>
       </c>
-      <c r="B225" s="44">
+      <c r="B225" s="40">
         <v>480</v>
       </c>
       <c r="C225" s="1" t="s">
@@ -4506,7 +4803,7 @@
         <f t="shared" si="1"/>
         <v>44328.999305555553</v>
       </c>
-      <c r="B226" s="44">
+      <c r="B226" s="40">
         <v>480</v>
       </c>
       <c r="C226" s="1" t="s">
@@ -4518,7 +4815,7 @@
         <f t="shared" si="1"/>
         <v>44329.999305555553</v>
       </c>
-      <c r="B227" s="44">
+      <c r="B227" s="40">
         <v>480</v>
       </c>
       <c r="C227" s="1" t="s">
@@ -4530,7 +4827,7 @@
         <f t="shared" si="1"/>
         <v>44330.999305555553</v>
       </c>
-      <c r="B228" s="44">
+      <c r="B228" s="40">
         <v>480</v>
       </c>
       <c r="C228" s="1" t="s">
@@ -4542,7 +4839,7 @@
         <f t="shared" si="1"/>
         <v>44331.999305555553</v>
       </c>
-      <c r="B229" s="44">
+      <c r="B229" s="40">
         <v>480</v>
       </c>
       <c r="C229" s="1" t="s">
@@ -4554,7 +4851,7 @@
         <f t="shared" si="1"/>
         <v>44332.999305555553</v>
       </c>
-      <c r="B230" s="44">
+      <c r="B230" s="40">
         <v>480</v>
       </c>
       <c r="C230" s="1" t="s">
@@ -4566,7 +4863,7 @@
         <f t="shared" si="1"/>
         <v>44333.999305555553</v>
       </c>
-      <c r="B231" s="44">
+      <c r="B231" s="40">
         <v>480</v>
       </c>
       <c r="C231" s="1" t="s">
@@ -4578,7 +4875,7 @@
         <f t="shared" si="1"/>
         <v>44334.999305555553</v>
       </c>
-      <c r="B232" s="44">
+      <c r="B232" s="40">
         <v>480</v>
       </c>
       <c r="C232" s="1" t="s">
@@ -4590,7 +4887,7 @@
         <f t="shared" si="1"/>
         <v>44335.999305555553</v>
       </c>
-      <c r="B233" s="44">
+      <c r="B233" s="40">
         <v>480</v>
       </c>
       <c r="C233" s="1" t="s">
@@ -4602,7 +4899,7 @@
         <f t="shared" si="1"/>
         <v>44336.999305555553</v>
       </c>
-      <c r="B234" s="44">
+      <c r="B234" s="40">
         <v>480</v>
       </c>
       <c r="C234" s="1" t="s">
@@ -4614,7 +4911,7 @@
         <f t="shared" si="1"/>
         <v>44337.999305555553</v>
       </c>
-      <c r="B235" s="44">
+      <c r="B235" s="40">
         <v>480</v>
       </c>
       <c r="C235" s="1" t="s">
@@ -4626,7 +4923,7 @@
         <f t="shared" si="1"/>
         <v>44338.999305555553</v>
       </c>
-      <c r="B236" s="44">
+      <c r="B236" s="40">
         <v>480</v>
       </c>
       <c r="C236" s="1" t="s">
@@ -4638,7 +4935,7 @@
         <f t="shared" si="1"/>
         <v>44339.999305555553</v>
       </c>
-      <c r="B237" s="44">
+      <c r="B237" s="40">
         <v>480</v>
       </c>
       <c r="C237" s="1" t="s">
@@ -4650,7 +4947,7 @@
         <f t="shared" si="1"/>
         <v>44340.999305555553</v>
       </c>
-      <c r="B238" s="44">
+      <c r="B238" s="40">
         <v>480</v>
       </c>
       <c r="C238" s="1" t="s">
@@ -4662,7 +4959,7 @@
         <f t="shared" si="1"/>
         <v>44341.999305555553</v>
       </c>
-      <c r="B239" s="44">
+      <c r="B239" s="40">
         <v>480</v>
       </c>
       <c r="C239" s="1" t="s">
@@ -4674,7 +4971,7 @@
         <f t="shared" si="1"/>
         <v>44342.999305555553</v>
       </c>
-      <c r="B240" s="44">
+      <c r="B240" s="40">
         <v>480</v>
       </c>
       <c r="C240" s="1" t="s">
@@ -4686,7 +4983,7 @@
         <f t="shared" si="1"/>
         <v>44343.999305555553</v>
       </c>
-      <c r="B241" s="44">
+      <c r="B241" s="40">
         <v>480</v>
       </c>
       <c r="C241" s="1" t="s">
@@ -4698,7 +4995,7 @@
         <f t="shared" si="1"/>
         <v>44344.999305555553</v>
       </c>
-      <c r="B242" s="44">
+      <c r="B242" s="40">
         <v>480</v>
       </c>
       <c r="C242" s="1" t="s">
@@ -4710,7 +5007,7 @@
         <f t="shared" si="1"/>
         <v>44345.999305555553</v>
       </c>
-      <c r="B243" s="44">
+      <c r="B243" s="40">
         <v>480</v>
       </c>
       <c r="C243" s="1" t="s">
@@ -4722,7 +5019,7 @@
         <f t="shared" si="1"/>
         <v>44346.999305555553</v>
       </c>
-      <c r="B244" s="44">
+      <c r="B244" s="40">
         <v>480</v>
       </c>
       <c r="C244" s="1" t="s">
@@ -4734,7 +5031,7 @@
         <f t="shared" si="1"/>
         <v>44347.999305555553</v>
       </c>
-      <c r="B245" s="44">
+      <c r="B245" s="40">
         <v>480</v>
       </c>
       <c r="C245" s="1" t="s">
@@ -4746,7 +5043,7 @@
         <f t="shared" si="1"/>
         <v>44348.999305555553</v>
       </c>
-      <c r="B246" s="44">
+      <c r="B246" s="40">
         <v>480</v>
       </c>
       <c r="C246" s="1" t="s">
@@ -4758,7 +5055,7 @@
         <f t="shared" si="1"/>
         <v>44349.999305555553</v>
       </c>
-      <c r="B247" s="44">
+      <c r="B247" s="40">
         <v>480</v>
       </c>
       <c r="C247" s="1" t="s">
@@ -4770,7 +5067,7 @@
         <f t="shared" si="1"/>
         <v>44350.999305555553</v>
       </c>
-      <c r="B248" s="44">
+      <c r="B248" s="40">
         <v>480</v>
       </c>
       <c r="C248" s="1" t="s">
@@ -4782,7 +5079,7 @@
         <f t="shared" si="1"/>
         <v>44351.999305555553</v>
       </c>
-      <c r="B249" s="44">
+      <c r="B249" s="40">
         <v>0</v>
       </c>
       <c r="C249" s="1" t="s">
@@ -8219,15 +8516,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BP6"/>
+  <dimension ref="A1:BR6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15.42578125" style="5" customWidth="1"/>
+    <col min="2" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="10.42578125" style="5" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="5"/>
     <col min="10" max="10" width="12.28515625" style="5" customWidth="1"/>
@@ -8237,7 +8535,7 @@
     <col min="14" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="32" customFormat="1" ht="339">
+    <row r="1" spans="1:70" s="32" customFormat="1" ht="339">
       <c r="B1" s="33" t="s">
         <v>121</v>
       </c>
@@ -8440,8 +8738,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:68">
-      <c r="A2" s="34">
+    <row r="2" spans="1:70">
+      <c r="A2" s="41">
         <v>-36522.000694444447</v>
       </c>
       <c r="B2" s="5">
@@ -8573,14 +8871,14 @@
       <c r="AR2" s="5">
         <v>12</v>
       </c>
-      <c r="AS2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AT2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AU2" s="5">
-        <v>0.9</v>
+      <c r="AS2" s="43">
+        <v>0.85</v>
+      </c>
+      <c r="AT2" s="43">
+        <v>0.85</v>
+      </c>
+      <c r="AU2" s="43">
+        <v>0.85</v>
       </c>
       <c r="AV2" s="5">
         <v>1</v>
@@ -8594,14 +8892,14 @@
       <c r="AY2" s="5">
         <v>12</v>
       </c>
-      <c r="AZ2" s="5">
+      <c r="AZ2" s="43">
         <v>0.8</v>
       </c>
-      <c r="BA2" s="5">
+      <c r="BA2" s="43">
         <v>0.8</v>
       </c>
-      <c r="BB2" s="5">
-        <v>0.9</v>
+      <c r="BB2" s="43">
+        <v>0.8</v>
       </c>
       <c r="BC2" s="5">
         <v>1</v>
@@ -8615,13 +8913,13 @@
       <c r="BF2" s="5">
         <v>12</v>
       </c>
-      <c r="BG2" s="5">
+      <c r="BG2" s="43">
         <v>0.75</v>
       </c>
-      <c r="BH2" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="BI2" s="5">
+      <c r="BH2" s="43">
+        <v>0.75</v>
+      </c>
+      <c r="BI2" s="43">
         <v>0.75</v>
       </c>
       <c r="BJ2" s="5">
@@ -8636,17 +8934,20 @@
       <c r="BM2" s="5">
         <v>12</v>
       </c>
-      <c r="BN2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="BO2" s="5">
+      <c r="BN2" s="43">
         <v>0.8</v>
       </c>
-      <c r="BP2" s="5">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:68">
+      <c r="BO2" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="BP2" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="BR2" s="45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:70">
       <c r="A3" s="34">
         <v>-36521.959027777775</v>
       </c>
@@ -8779,14 +9080,14 @@
       <c r="AR3" s="5">
         <v>12</v>
       </c>
-      <c r="AS3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AT3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AU3" s="5">
-        <v>0.9</v>
+      <c r="AS3" s="43">
+        <v>0.95</v>
+      </c>
+      <c r="AT3" s="43">
+        <v>0.95</v>
+      </c>
+      <c r="AU3" s="43">
+        <v>0.95</v>
       </c>
       <c r="AV3" s="5">
         <v>1</v>
@@ -8800,13 +9101,13 @@
       <c r="AY3" s="5">
         <v>12</v>
       </c>
-      <c r="AZ3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BA3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BB3" s="5">
+      <c r="AZ3" s="43">
+        <v>0.9</v>
+      </c>
+      <c r="BA3" s="43">
+        <v>0.9</v>
+      </c>
+      <c r="BB3" s="43">
         <v>0.9</v>
       </c>
       <c r="BC3" s="5">
@@ -8821,14 +9122,14 @@
       <c r="BF3" s="5">
         <v>12</v>
       </c>
-      <c r="BG3" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="BH3" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="BI3" s="5">
-        <v>0.75</v>
+      <c r="BG3" s="43">
+        <v>0.85</v>
+      </c>
+      <c r="BH3" s="43">
+        <v>0.85</v>
+      </c>
+      <c r="BI3" s="43">
+        <v>0.85</v>
       </c>
       <c r="BJ3" s="5">
         <v>1</v>
@@ -8842,17 +9143,20 @@
       <c r="BM3" s="5">
         <v>12</v>
       </c>
-      <c r="BN3" s="5">
+      <c r="BN3" s="43">
         <v>0.9</v>
       </c>
-      <c r="BO3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BP3" s="5">
+      <c r="BO3" s="43">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:68">
+      <c r="BP3" s="43">
+        <v>0.9</v>
+      </c>
+      <c r="BR3" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:70">
       <c r="A4" s="34">
         <v>-36521.917361111111</v>
       </c>
@@ -8985,14 +9289,14 @@
       <c r="AR4" s="5">
         <v>12</v>
       </c>
-      <c r="AS4" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AT4" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AU4" s="5">
-        <v>0.9</v>
+      <c r="AS4" s="43">
+        <v>0.75</v>
+      </c>
+      <c r="AT4" s="43">
+        <v>0.75</v>
+      </c>
+      <c r="AU4" s="43">
+        <v>0.75</v>
       </c>
       <c r="AV4" s="5">
         <v>1</v>
@@ -9006,14 +9310,14 @@
       <c r="AY4" s="5">
         <v>12</v>
       </c>
-      <c r="AZ4" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BA4" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BB4" s="5">
-        <v>0.9</v>
+      <c r="AZ4" s="43">
+        <v>0.7</v>
+      </c>
+      <c r="BA4" s="43">
+        <v>0.7</v>
+      </c>
+      <c r="BB4" s="43">
+        <v>0.7</v>
       </c>
       <c r="BC4" s="5">
         <v>1</v>
@@ -9027,14 +9331,14 @@
       <c r="BF4" s="5">
         <v>12</v>
       </c>
-      <c r="BG4" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="BH4" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="BI4" s="5">
-        <v>0.75</v>
+      <c r="BG4" s="43">
+        <v>0.65</v>
+      </c>
+      <c r="BH4" s="43">
+        <v>0.65</v>
+      </c>
+      <c r="BI4" s="43">
+        <v>0.65</v>
       </c>
       <c r="BJ4" s="5">
         <v>1</v>
@@ -9048,17 +9352,20 @@
       <c r="BM4" s="5">
         <v>12</v>
       </c>
-      <c r="BN4" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="BO4" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BP4" s="5">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:68">
+      <c r="BN4" s="43">
+        <v>0.7</v>
+      </c>
+      <c r="BO4" s="43">
+        <v>0.7</v>
+      </c>
+      <c r="BP4" s="43">
+        <v>0.7</v>
+      </c>
+      <c r="BR4" s="45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:70">
       <c r="A5" s="34">
         <v>-36521.875694444447</v>
       </c>
@@ -9191,14 +9498,14 @@
       <c r="AR5" s="5">
         <v>12</v>
       </c>
-      <c r="AS5" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AT5" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="AU5" s="5">
-        <v>0.9</v>
+      <c r="AS5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="AT5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="AU5" s="43">
+        <v>0.5</v>
       </c>
       <c r="AV5" s="5">
         <v>1</v>
@@ -9212,14 +9519,14 @@
       <c r="AY5" s="5">
         <v>12</v>
       </c>
-      <c r="AZ5" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BA5" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BB5" s="5">
-        <v>0.9</v>
+      <c r="AZ5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="BA5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="BB5" s="43">
+        <v>0.5</v>
       </c>
       <c r="BC5" s="5">
         <v>1</v>
@@ -9233,14 +9540,14 @@
       <c r="BF5" s="5">
         <v>12</v>
       </c>
-      <c r="BG5" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="BH5" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="BI5" s="5">
-        <v>0.75</v>
+      <c r="BG5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="BH5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="BI5" s="43">
+        <v>0.5</v>
       </c>
       <c r="BJ5" s="5">
         <v>1</v>
@@ -9254,17 +9561,20 @@
       <c r="BM5" s="5">
         <v>12</v>
       </c>
-      <c r="BN5" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="BO5" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="BP5" s="5">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:68">
+      <c r="BN5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="BO5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="BP5" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="BR5" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:70">
       <c r="A6" s="34">
         <v>-36521.834027777775</v>
       </c>
@@ -9397,13 +9707,13 @@
       <c r="AR6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="AS6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="36" t="s">
+      <c r="AS6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="44" t="s">
         <v>1</v>
       </c>
       <c r="AV6" s="36" t="s">
@@ -9418,13 +9728,13 @@
       <c r="AY6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="AZ6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB6" s="36" t="s">
+      <c r="AZ6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB6" s="44" t="s">
         <v>1</v>
       </c>
       <c r="BC6" s="36" t="s">
@@ -9439,13 +9749,13 @@
       <c r="BF6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="BG6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="BH6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="BI6" s="36" t="s">
+      <c r="BG6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI6" s="44" t="s">
         <v>1</v>
       </c>
       <c r="BJ6" s="36" t="s">
@@ -9460,13 +9770,13 @@
       <c r="BM6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="BN6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="BO6" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="BP6" s="36" t="s">
+      <c r="BN6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO6" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="BP6" s="44" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed name of NRCS and CNRFC slots
Changed the names of two slots on the workspace:
Forecasts.CNRFC Percentile Forecasts for Comparison to "CNRFC Forecasts for Comparison"
Forecasts.NRCS Percentile Forecasts for Comparison to "NRCS Forecasts for Comparison"

I also updated RPL logic, DMI's (including the 2021WY spreadsheet) and Output devices.
</commit_message>
<xml_diff>
--- a/Database/KPOM_OM_InputsForTesting.xlsx
+++ b/Database/KPOM_OM_InputsForTesting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\riverware\staff\neumannd\KROM\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\riverware\staff\neumannd\KPOM\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1356399-75F2-4DAC-869D-67BDA4B0C74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E699A74-C9BA-4198-BFEA-A1E9756E47CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="1860" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="2595" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="2" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="133">
   <si>
     <t>EWA.EWA May June Augment Release</t>
   </si>
@@ -184,9 +184,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>Forecasts.NRCS Percentile Forecasts for Comparison</t>
-  </si>
-  <si>
     <t>30th</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>70th</t>
   </si>
   <si>
-    <t>Forecasts.CNRFC Percentile Forecasts for Comparison</t>
-  </si>
-  <si>
     <t>25th</t>
   </si>
   <si>
@@ -478,9 +472,6 @@
     <t>MRM Dashboard.Agricultural Date Settings.Short</t>
   </si>
   <si>
-    <t>We should replace "Percentile" to "POE", "EP", or something that indicates exceedance instead of percentile</t>
-  </si>
-  <si>
     <t>! median accretion</t>
   </si>
   <si>
@@ -494,6 +485,12 @@
   </si>
   <si>
     <t>Nan</t>
+  </si>
+  <si>
+    <t>Forecasts.NRCS Forecasts for Comparison</t>
+  </si>
+  <si>
+    <t>Forecasts.CNRFC Forecasts for Comparison</t>
   </si>
 </sst>
 </file>
@@ -800,6 +797,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -808,12 +811,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,255 +827,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1171575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C8A6BB6-7C7C-44E9-AA3B-E4A2F3E3968E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8982075" y="171450"/>
-          <a:ext cx="247650" cy="2628900"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E691EA-8BD0-4B6C-A2A8-7284122758D4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9324975" y="180975"/>
-          <a:ext cx="2457450" cy="2600325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79EB9EF1-310B-44DF-A2BD-4D4DF8232C12}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8543925" y="9525"/>
-          <a:ext cx="676275" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27117716-AE17-4C08-8405-FDA568F4AA5B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11458575" y="9525"/>
-          <a:ext cx="676275" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1380,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1427,112 +1175,112 @@
   <sheetData>
     <row r="1" spans="1:41">
       <c r="A1" s="8"/>
-      <c r="B1" s="48" t="s">
-        <v>41</v>
+      <c r="B1" s="50" t="s">
+        <v>39</v>
       </c>
       <c r="C1" s="8"/>
-      <c r="D1" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="47"/>
+      <c r="D1" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
+      <c r="I1" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
       <c r="M1" s="8"/>
-      <c r="N1" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="47"/>
+      <c r="N1" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="49"/>
       <c r="R1" s="20" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="8"/>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="46"/>
+      <c r="U1" s="48"/>
       <c r="V1" s="8"/>
-      <c r="W1" s="46" t="s">
+      <c r="W1" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="47"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="49"/>
       <c r="Z1" s="8"/>
-      <c r="AA1" s="46" t="s">
+      <c r="AA1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="47"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="49"/>
       <c r="AD1" s="8"/>
-      <c r="AE1" s="46" t="s">
+      <c r="AE1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="47"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="49"/>
       <c r="AH1" s="8"/>
-      <c r="AI1" s="46" t="s">
+      <c r="AI1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="47"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="49"/>
       <c r="AL1" s="8"/>
-      <c r="AM1" s="46" t="s">
+      <c r="AM1" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="47"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="49"/>
     </row>
     <row r="2" spans="1:41">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R2" s="12">
         <v>140000</v>
@@ -1597,7 +1345,7 @@
     </row>
     <row r="3" spans="1:41">
       <c r="A3" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
@@ -1720,7 +1468,7 @@
     </row>
     <row r="4" spans="1:41">
       <c r="A4" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -1799,7 +1547,7 @@
     </row>
     <row r="5" spans="1:41">
       <c r="A5" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="11">
         <v>0.33</v>
@@ -1812,10 +1560,10 @@
       <c r="F5" s="16"/>
       <c r="G5" s="11"/>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R5" s="16"/>
       <c r="S5" s="14" t="s">
@@ -1884,7 +1632,7 @@
     </row>
     <row r="6" spans="1:41">
       <c r="A6" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="11">
         <v>0.35</v>
@@ -1915,7 +1663,7 @@
     </row>
     <row r="7" spans="1:41">
       <c r="A7" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="11">
         <v>0.34</v>
@@ -1946,7 +1694,7 @@
     </row>
     <row r="8" spans="1:41">
       <c r="A8" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="11">
         <v>0.47</v>
@@ -1977,7 +1725,7 @@
     </row>
     <row r="9" spans="1:41">
       <c r="A9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="11">
         <v>0.47</v>
@@ -1999,7 +1747,7 @@
     </row>
     <row r="10" spans="1:41">
       <c r="A10" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="11">
         <v>0.47</v>
@@ -2007,21 +1755,21 @@
     </row>
     <row r="11" spans="1:41">
       <c r="A11" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="11">
         <v>0.47</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="W11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:41">
       <c r="A12" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="11">
         <v>0.5</v>
@@ -2029,7 +1777,7 @@
     </row>
     <row r="13" spans="1:41">
       <c r="A13" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="11">
         <v>0.5</v>
@@ -2039,7 +1787,7 @@
     </row>
     <row r="14" spans="1:41">
       <c r="A14" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="11">
         <v>0.5</v>
@@ -2049,7 +1797,7 @@
     </row>
     <row r="15" spans="1:41">
       <c r="A15" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="11">
         <v>0.5</v>
@@ -2059,20 +1807,18 @@
     </row>
     <row r="16" spans="1:41">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" s="11">
         <v>0.46</v>
       </c>
       <c r="C16" s="5"/>
       <c r="E16" s="7"/>
-      <c r="J16" s="42" t="s">
-        <v>128</v>
-      </c>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" s="13">
         <v>0.46</v>
@@ -2090,14 +1836,14 @@
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="5"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>0.52</v>
@@ -2107,7 +1853,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>0.52</v>
@@ -2115,7 +1861,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>0.52</v>
@@ -2123,7 +1869,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24">
         <v>0.52</v>
@@ -2131,7 +1877,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>0.52</v>
@@ -2139,7 +1885,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>0.52</v>
@@ -2147,7 +1893,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B27">
         <v>0.52</v>
@@ -2155,7 +1901,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28">
         <v>0.52</v>
@@ -2163,7 +1909,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29">
         <v>0.53</v>
@@ -2171,7 +1917,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>0.52</v>
@@ -2179,7 +1925,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>0.52</v>
@@ -2187,7 +1933,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32">
         <v>0.53</v>
@@ -2195,7 +1941,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B33">
         <v>0.36</v>
@@ -2203,7 +1949,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B34">
         <v>0.36</v>
@@ -2211,7 +1957,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2219,19 +1965,18 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B1"/>
+    <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AE1:AG1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B1"/>
-    <mergeCell ref="AA1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2239,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C520"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B194" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4470,7 +4215,7 @@
       <c r="B198" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C198" s="49" t="s">
+      <c r="C198" s="46" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4518,8 +4263,8 @@
       <c r="B202" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C202" s="50" t="s">
-        <v>133</v>
+      <c r="C202" s="47" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -8344,7 +8089,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -8537,205 +8282,205 @@
   <sheetData>
     <row r="1" spans="1:70" s="32" customFormat="1" ht="339">
       <c r="B1" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="J1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>125</v>
-      </c>
       <c r="N1" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="S1" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="T1" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AB1" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AD1" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="AC1" s="33" t="s">
+      <c r="AE1" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="AD1" s="33" t="s">
+      <c r="AF1" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AG1" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AH1" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="AH1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="AI1" s="33" t="s">
+      <c r="AK1" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="AJ1" s="33" t="s">
+      <c r="AL1" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="AK1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="AM1" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN1" s="33" t="s">
-        <v>115</v>
-      </c>
       <c r="AO1" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ1" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="AP1" s="33" t="s">
+      <c r="AR1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="AQ1" s="33" t="s">
+      <c r="AS1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="AR1" s="33" t="s">
+      <c r="AT1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="AS1" s="33" t="s">
+      <c r="AU1" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="AT1" s="33" t="s">
+      <c r="AV1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="AU1" s="33" t="s">
+      <c r="AW1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="AV1" s="33" t="s">
+      <c r="AX1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="AW1" s="33" t="s">
+      <c r="AY1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="AX1" s="33" t="s">
+      <c r="AZ1" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="AY1" s="33" t="s">
+      <c r="BA1" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="AZ1" s="33" t="s">
+      <c r="BB1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="BA1" s="33" t="s">
+      <c r="BC1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="BB1" s="33" t="s">
+      <c r="BD1" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="BC1" s="33" t="s">
+      <c r="BE1" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="BD1" s="33" t="s">
+      <c r="BF1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="BE1" s="33" t="s">
+      <c r="BG1" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="BF1" s="33" t="s">
+      <c r="BH1" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="BG1" s="33" t="s">
+      <c r="BI1" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="BH1" s="33" t="s">
+      <c r="BJ1" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="BI1" s="33" t="s">
+      <c r="BK1" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="33" t="s">
+      <c r="BL1" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="BK1" s="33" t="s">
+      <c r="BM1" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="BL1" s="33" t="s">
+      <c r="BN1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="BM1" s="33" t="s">
+      <c r="BO1" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="BN1" s="33" t="s">
+      <c r="BP1" s="33" t="s">
         <v>86</v>
-      </c>
-      <c r="BO1" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="BP1" s="33" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:70">
@@ -8944,7 +8689,7 @@
         <v>0.8</v>
       </c>
       <c r="BR2" s="45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:70">
@@ -9153,7 +8898,7 @@
         <v>0.9</v>
       </c>
       <c r="BR3" s="45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:70">
@@ -9362,7 +9107,7 @@
         <v>0.7</v>
       </c>
       <c r="BR4" s="45" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:70">
@@ -9571,7 +9316,7 @@
         <v>0.5</v>
       </c>
       <c r="BR5" s="45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:70">

</xml_diff>